<commit_message>
Finished 3cm curvature analysis for 2015
</commit_message>
<xml_diff>
--- a/data/GIS_MPQ_Analysis_3cm_Curvature.xlsx
+++ b/data/GIS_MPQ_Analysis_3cm_Curvature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="240" windowWidth="25600" windowHeight="11640" tabRatio="500"/>
+    <workbookView xWindow="29180" yWindow="220" windowWidth="21740" windowHeight="11640" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Curvature" sheetId="2" r:id="rId1"/>
@@ -126,8 +126,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -206,6 +264,35 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -229,6 +316,35 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1062,8 +1178,29 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>22096</v>
+      </c>
+      <c r="E16">
+        <v>19.886399999999998</v>
+      </c>
+      <c r="F16">
+        <v>-113057.5625</v>
+      </c>
+      <c r="G16">
+        <v>94997.0625</v>
+      </c>
+      <c r="H16">
+        <v>208054.625</v>
+      </c>
+      <c r="I16">
+        <v>20.760270999999999</v>
+      </c>
+      <c r="J16">
+        <v>9277.4813969999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1073,8 +1210,29 @@
       <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>22314</v>
+      </c>
+      <c r="E17">
+        <v>20.082599999999999</v>
+      </c>
+      <c r="F17">
+        <v>-79605</v>
+      </c>
+      <c r="G17">
+        <v>50441.476562999997</v>
+      </c>
+      <c r="H17">
+        <v>130046.476563</v>
+      </c>
+      <c r="I17">
+        <v>4.2869099999999998</v>
+      </c>
+      <c r="J17">
+        <v>6726.4234059999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1084,8 +1242,29 @@
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>16131</v>
+      </c>
+      <c r="E18">
+        <v>14.517899999999999</v>
+      </c>
+      <c r="F18">
+        <v>-48516.960937999997</v>
+      </c>
+      <c r="G18">
+        <v>44731.777344000002</v>
+      </c>
+      <c r="H18">
+        <v>93248.738280999998</v>
+      </c>
+      <c r="I18">
+        <v>-12.991279</v>
+      </c>
+      <c r="J18">
+        <v>6157.7164089999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1095,8 +1274,29 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>19415</v>
+      </c>
+      <c r="E19">
+        <v>17.473500000000001</v>
+      </c>
+      <c r="F19">
+        <v>-92679.898438000004</v>
+      </c>
+      <c r="G19">
+        <v>93582.601563000004</v>
+      </c>
+      <c r="H19">
+        <v>186262.5</v>
+      </c>
+      <c r="I19">
+        <v>-1.1193040000000001</v>
+      </c>
+      <c r="J19">
+        <v>9120.9722089999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1106,8 +1306,29 @@
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>18835</v>
+      </c>
+      <c r="E20">
+        <v>16.951499999999999</v>
+      </c>
+      <c r="F20">
+        <v>-78936.125</v>
+      </c>
+      <c r="G20">
+        <v>119264.101563</v>
+      </c>
+      <c r="H20">
+        <v>198200.226563</v>
+      </c>
+      <c r="I20">
+        <v>19.950292999999999</v>
+      </c>
+      <c r="J20">
+        <v>8421.8076760000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1117,8 +1338,29 @@
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>21400</v>
+      </c>
+      <c r="E21">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="F21">
+        <v>-143074.25</v>
+      </c>
+      <c r="G21">
+        <v>105557.46875</v>
+      </c>
+      <c r="H21">
+        <v>248631.71875</v>
+      </c>
+      <c r="I21">
+        <v>14.081272</v>
+      </c>
+      <c r="J21">
+        <v>9108.5376219999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1128,8 +1370,29 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>18613</v>
+      </c>
+      <c r="E22">
+        <v>16.7517</v>
+      </c>
+      <c r="F22">
+        <v>-64001.746094000002</v>
+      </c>
+      <c r="G22">
+        <v>58183.300780999998</v>
+      </c>
+      <c r="H22">
+        <v>122185.046875</v>
+      </c>
+      <c r="I22">
+        <v>22.793627999999998</v>
+      </c>
+      <c r="J22">
+        <v>6006.4417119999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1139,8 +1402,29 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>19843</v>
+      </c>
+      <c r="E23">
+        <v>17.858699999999999</v>
+      </c>
+      <c r="F23">
+        <v>-94722.539063000004</v>
+      </c>
+      <c r="G23">
+        <v>82953.867188000004</v>
+      </c>
+      <c r="H23">
+        <v>177676.40625</v>
+      </c>
+      <c r="I23">
+        <v>19.693408000000002</v>
+      </c>
+      <c r="J23">
+        <v>8616.8592590000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1149,6 +1433,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="D24">
+        <v>18845</v>
+      </c>
+      <c r="E24">
+        <v>16.9605</v>
+      </c>
+      <c r="F24">
+        <v>-177645.546875</v>
+      </c>
+      <c r="G24">
+        <v>120519.875</v>
+      </c>
+      <c r="H24">
+        <v>298165.421875</v>
+      </c>
+      <c r="I24">
+        <v>32.655202000000003</v>
+      </c>
+      <c r="J24">
+        <v>12259.073715</v>
       </c>
     </row>
   </sheetData>
@@ -1166,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1668,8 +1973,29 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>22096</v>
+      </c>
+      <c r="E16">
+        <v>19.886399999999998</v>
+      </c>
+      <c r="F16">
+        <v>-77939.507813000004</v>
+      </c>
+      <c r="G16">
+        <v>63492.152344000002</v>
+      </c>
+      <c r="H16">
+        <v>141431.660156</v>
+      </c>
+      <c r="I16">
+        <v>87.873146000000006</v>
+      </c>
+      <c r="J16">
+        <v>4347.5604960000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1679,8 +2005,29 @@
       <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>22314</v>
+      </c>
+      <c r="E17">
+        <v>20.082599999999999</v>
+      </c>
+      <c r="F17">
+        <v>-37430.941405999998</v>
+      </c>
+      <c r="G17">
+        <v>26780.464843999998</v>
+      </c>
+      <c r="H17">
+        <v>64211.40625</v>
+      </c>
+      <c r="I17">
+        <v>124.46781799999999</v>
+      </c>
+      <c r="J17">
+        <v>3261.4611169999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1690,8 +2037,29 @@
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>16131</v>
+      </c>
+      <c r="E18">
+        <v>14.517899999999999</v>
+      </c>
+      <c r="F18">
+        <v>-35157.300780999998</v>
+      </c>
+      <c r="G18">
+        <v>26354.185547000001</v>
+      </c>
+      <c r="H18">
+        <v>61511.486327999999</v>
+      </c>
+      <c r="I18">
+        <v>132.71728300000001</v>
+      </c>
+      <c r="J18">
+        <v>2951.3188719999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1701,8 +2069,29 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>19415</v>
+      </c>
+      <c r="E19">
+        <v>17.473500000000001</v>
+      </c>
+      <c r="F19">
+        <v>-53631.550780999998</v>
+      </c>
+      <c r="G19">
+        <v>51617.335937999997</v>
+      </c>
+      <c r="H19">
+        <v>105248.886719</v>
+      </c>
+      <c r="I19">
+        <v>107.79254299999999</v>
+      </c>
+      <c r="J19">
+        <v>4334.7871660000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1712,8 +2101,29 @@
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>18835</v>
+      </c>
+      <c r="E20">
+        <v>16.951499999999999</v>
+      </c>
+      <c r="F20">
+        <v>-38377.035155999998</v>
+      </c>
+      <c r="G20">
+        <v>57585.492187999997</v>
+      </c>
+      <c r="H20">
+        <v>95962.527344000002</v>
+      </c>
+      <c r="I20">
+        <v>113.21618100000001</v>
+      </c>
+      <c r="J20">
+        <v>4045.466488</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1723,8 +2133,29 @@
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>21400</v>
+      </c>
+      <c r="E21">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="F21">
+        <v>-76341.359375</v>
+      </c>
+      <c r="G21">
+        <v>62465.328125</v>
+      </c>
+      <c r="H21">
+        <v>138806.6875</v>
+      </c>
+      <c r="I21">
+        <v>122.871897</v>
+      </c>
+      <c r="J21">
+        <v>4395.6796850000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1734,8 +2165,29 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>18613</v>
+      </c>
+      <c r="E22">
+        <v>16.7517</v>
+      </c>
+      <c r="F22">
+        <v>-31937.058593999998</v>
+      </c>
+      <c r="G22">
+        <v>30746.246093999998</v>
+      </c>
+      <c r="H22">
+        <v>62683.304687999997</v>
+      </c>
+      <c r="I22">
+        <v>99.529325999999998</v>
+      </c>
+      <c r="J22">
+        <v>2766.8014210000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1745,8 +2197,29 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>19843</v>
+      </c>
+      <c r="E23">
+        <v>17.858699999999999</v>
+      </c>
+      <c r="F23">
+        <v>-54001.914062999997</v>
+      </c>
+      <c r="G23">
+        <v>59129.773437999997</v>
+      </c>
+      <c r="H23">
+        <v>113131.6875</v>
+      </c>
+      <c r="I23">
+        <v>136.55813599999999</v>
+      </c>
+      <c r="J23">
+        <v>4023.072885</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1755,6 +2228,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="D24">
+        <v>18845</v>
+      </c>
+      <c r="E24">
+        <v>16.9605</v>
+      </c>
+      <c r="F24">
+        <v>-111126.960938</v>
+      </c>
+      <c r="G24">
+        <v>91346.828125</v>
+      </c>
+      <c r="H24">
+        <v>202473.789063</v>
+      </c>
+      <c r="I24">
+        <v>46.561487</v>
+      </c>
+      <c r="J24">
+        <v>5972.5656269999999</v>
       </c>
     </row>
   </sheetData>
@@ -1772,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2275,8 +2769,29 @@
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>22096</v>
+      </c>
+      <c r="E16">
+        <v>19.886399999999998</v>
+      </c>
+      <c r="F16">
+        <v>-61546.707030999998</v>
+      </c>
+      <c r="G16">
+        <v>62662.535155999998</v>
+      </c>
+      <c r="H16">
+        <v>124209.242188</v>
+      </c>
+      <c r="I16">
+        <v>67.112870999999998</v>
+      </c>
+      <c r="J16">
+        <v>6063.3135350000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2286,8 +2801,29 @@
       <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>22314</v>
+      </c>
+      <c r="E17">
+        <v>20.082599999999999</v>
+      </c>
+      <c r="F17">
+        <v>-33802.496094000002</v>
+      </c>
+      <c r="G17">
+        <v>42174.054687999997</v>
+      </c>
+      <c r="H17">
+        <v>75976.550780999998</v>
+      </c>
+      <c r="I17">
+        <v>120.180908</v>
+      </c>
+      <c r="J17">
+        <v>4283.4623220000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2297,8 +2833,29 @@
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>16131</v>
+      </c>
+      <c r="E18">
+        <v>14.517899999999999</v>
+      </c>
+      <c r="F18">
+        <v>-24172.005859000001</v>
+      </c>
+      <c r="G18">
+        <v>28797.314452999999</v>
+      </c>
+      <c r="H18">
+        <v>52969.320312999997</v>
+      </c>
+      <c r="I18">
+        <v>145.708564</v>
+      </c>
+      <c r="J18">
+        <v>3973.0706340000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2308,8 +2865,29 @@
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>19415</v>
+      </c>
+      <c r="E19">
+        <v>17.473500000000001</v>
+      </c>
+      <c r="F19">
+        <v>-52245.726562999997</v>
+      </c>
+      <c r="G19">
+        <v>48715.410155999998</v>
+      </c>
+      <c r="H19">
+        <v>100961.136719</v>
+      </c>
+      <c r="I19">
+        <v>108.91184699999999</v>
+      </c>
+      <c r="J19">
+        <v>5881.8981130000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2319,8 +2897,29 @@
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>18835</v>
+      </c>
+      <c r="E20">
+        <v>16.951499999999999</v>
+      </c>
+      <c r="F20">
+        <v>-61678.605469000002</v>
+      </c>
+      <c r="G20">
+        <v>40559.089844000002</v>
+      </c>
+      <c r="H20">
+        <v>102237.695313</v>
+      </c>
+      <c r="I20">
+        <v>93.265889000000001</v>
+      </c>
+      <c r="J20">
+        <v>5405.6438870000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2330,8 +2929,29 @@
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>21400</v>
+      </c>
+      <c r="E21">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="F21">
+        <v>-60859.414062999997</v>
+      </c>
+      <c r="G21">
+        <v>66732.890625</v>
+      </c>
+      <c r="H21">
+        <v>127592.304688</v>
+      </c>
+      <c r="I21">
+        <v>108.79062500000001</v>
+      </c>
+      <c r="J21">
+        <v>5818.3414240000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2341,8 +2961,29 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>18613</v>
+      </c>
+      <c r="E22">
+        <v>16.7517</v>
+      </c>
+      <c r="F22">
+        <v>-39631.742187999997</v>
+      </c>
+      <c r="G22">
+        <v>48100.265625</v>
+      </c>
+      <c r="H22">
+        <v>87732.007813000004</v>
+      </c>
+      <c r="I22">
+        <v>76.735697000000002</v>
+      </c>
+      <c r="J22">
+        <v>4036.4183560000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2352,8 +2993,29 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>19843</v>
+      </c>
+      <c r="E23">
+        <v>17.858699999999999</v>
+      </c>
+      <c r="F23">
+        <v>-47754.503905999998</v>
+      </c>
+      <c r="G23">
+        <v>47029.464844000002</v>
+      </c>
+      <c r="H23">
+        <v>94783.96875</v>
+      </c>
+      <c r="I23">
+        <v>116.86472500000001</v>
+      </c>
+      <c r="J23">
+        <v>5743.853521</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2362,6 +3024,27 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="D24">
+        <v>18845</v>
+      </c>
+      <c r="E24">
+        <v>16.9605</v>
+      </c>
+      <c r="F24">
+        <v>-59257.761719000002</v>
+      </c>
+      <c r="G24">
+        <v>84534.875</v>
+      </c>
+      <c r="H24">
+        <v>143792.636719</v>
+      </c>
+      <c r="I24">
+        <v>13.906283999999999</v>
+      </c>
+      <c r="J24">
+        <v>7789.2204760000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>